<commit_message>
set up updated sim 1 (with small R2=.02)
</commit_message>
<xml_diff>
--- a/Variable naming conventions.xlsx
+++ b/Variable naming conventions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anita's Documents\MSc Utrecht\Master Thesis\01_MasterThesis_BES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2814FC-FE06-4F38-8A0C-00695D38913E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BA0F37-3355-4377-8ED1-32227AE07448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>3D array with BFs (rows=iterations, cols=studies, slices=conditions)</t>
   </si>
@@ -138,9 +138,6 @@
     <t>table that relates the power level to sample size</t>
   </si>
   <si>
-    <t>SDS</t>
-  </si>
-  <si>
     <t>k4</t>
   </si>
   <si>
@@ -160,13 +157,34 @@
   </si>
   <si>
     <t>rho= 0.1</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>exact replications</t>
+  </si>
+  <si>
+    <t>only linear regression</t>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>conceptual replications</t>
+  </si>
+  <si>
+    <t>linear, logistic, probit regression</t>
+  </si>
+  <si>
+    <t>concept</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +194,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,8 +226,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="F36:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +588,7 @@
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -594,17 +620,17 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>3</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
-        <v>38</v>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -640,7 +666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -651,7 +677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -662,7 +688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -673,56 +699,81 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>